<commit_message>
Adiciona CS_Consorcio_Contemplado.py ao processo de extração
</commit_message>
<xml_diff>
--- a/scraper-completo/DADOS EXTRAIDOS/extracao_SP_contemplados.xlsx
+++ b/scraper-completo/DADOS EXTRAIDOS/extracao_SP_contemplados.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -516,16 +516,16 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>54100,00</t>
+          <t>53730,00</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>28605,00</t>
+          <t>29586,50</t>
         </is>
       </c>
       <c r="E2" s="3" t="n">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
@@ -539,12 +539,12 @@
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>160 x R$ 369,97</t>
+          <t>163 x R$ 378,00</t>
         </is>
       </c>
       <c r="I2" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J2" s="3" t="inlineStr"/>
@@ -567,11 +567,11 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>33925,00</t>
+          <t>32925,00</t>
         </is>
       </c>
       <c r="E3" s="3" t="n">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
@@ -585,12 +585,12 @@
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>148 x R$ 415,00</t>
+          <t>158 x R$ 362,00</t>
         </is>
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr"/>
@@ -608,20 +608,20 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>65170,00</t>
+          <t>69750,00</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>32158,50</t>
+          <t>38387,50</t>
         </is>
       </c>
       <c r="E4" s="3" t="n">
-        <v>219</v>
+        <v>138</v>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G4" s="3" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="H4" s="3" t="inlineStr">
         <is>
-          <t>219 x R$ 339,69</t>
+          <t>138 x R$ 486,00</t>
         </is>
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J4" s="3" t="inlineStr"/>
@@ -654,16 +654,16 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>71200,00</t>
+          <t>70000,00</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>33060,00</t>
+          <t>41400,00</t>
         </is>
       </c>
       <c r="E5" s="3" t="n">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
@@ -672,17 +672,17 @@
       </c>
       <c r="G5" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H5" s="3" t="inlineStr">
         <is>
-          <t>148 x R$ 454,00</t>
+          <t>192 x R$ 378,00</t>
         </is>
       </c>
       <c r="I5" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J5" s="3" t="inlineStr"/>
@@ -700,16 +700,16 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>73400,00</t>
+          <t>70230,00</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>29670,00</t>
+          <t>38511,50</t>
         </is>
       </c>
       <c r="E6" s="3" t="n">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
@@ -718,17 +718,17 @@
       </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H6" s="3" t="inlineStr">
         <is>
-          <t>183 x R$ 478,62</t>
+          <t>191 x R$ 471,00</t>
         </is>
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J6" s="3" t="inlineStr"/>
@@ -746,16 +746,16 @@
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>78600,00</t>
+          <t>70300,00</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>53920,00</t>
+          <t>38415,00</t>
         </is>
       </c>
       <c r="E7" s="3" t="n">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
@@ -769,12 +769,12 @@
       </c>
       <c r="H7" s="3" t="inlineStr">
         <is>
-          <t>155 x R$ 406,00</t>
+          <t>192 x R$ 470,00</t>
         </is>
       </c>
       <c r="I7" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J7" s="3" t="inlineStr"/>
@@ -792,16 +792,16 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>79000,00</t>
+          <t>71154,00</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>50850,00</t>
+          <t>32529,70</t>
         </is>
       </c>
       <c r="E8" s="3" t="n">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="F8" s="3" t="inlineStr">
         <is>
@@ -810,17 +810,17 @@
       </c>
       <c r="G8" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H8" s="3" t="inlineStr">
         <is>
-          <t>154 x R$ 435,00</t>
+          <t>192 x R$ 472,00</t>
         </is>
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J8" s="3" t="inlineStr"/>
@@ -838,16 +838,16 @@
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>84526,69</t>
+          <t>71350,00</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>44126,33</t>
+          <t>38567,50</t>
         </is>
       </c>
       <c r="E9" s="3" t="n">
-        <v>126</v>
+        <v>191</v>
       </c>
       <c r="F9" s="3" t="inlineStr">
         <is>
@@ -861,12 +861,12 @@
       </c>
       <c r="H9" s="3" t="inlineStr">
         <is>
-          <t>126 x R$ 729,03</t>
+          <t>191 x R$ 472,00</t>
         </is>
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J9" s="3" t="inlineStr"/>
@@ -884,20 +884,20 @@
       </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
-          <t>85500,00</t>
+          <t>79700,00</t>
         </is>
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>45775,00</t>
+          <t>40885,00</t>
         </is>
       </c>
       <c r="E10" s="3" t="n">
-        <v>112</v>
+        <v>163</v>
       </c>
       <c r="F10" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G10" s="3" t="inlineStr">
@@ -907,12 +907,12 @@
       </c>
       <c r="H10" s="3" t="inlineStr">
         <is>
-          <t>112 x R$ 588,00</t>
+          <t>163 x R$ 560,00</t>
         </is>
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J10" s="3" t="inlineStr"/>
@@ -930,16 +930,16 @@
       </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t>87643,69</t>
+          <t>82980,00</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>46282,18</t>
+          <t>40849,00</t>
         </is>
       </c>
       <c r="E11" s="3" t="n">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="F11" s="3" t="inlineStr">
         <is>
@@ -953,12 +953,12 @@
       </c>
       <c r="H11" s="3" t="inlineStr">
         <is>
-          <t>109 x R$ 872,00</t>
+          <t>133 x R$ 723,00</t>
         </is>
       </c>
       <c r="I11" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J11" s="3" t="inlineStr"/>
@@ -976,16 +976,16 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>88700,00</t>
+          <t>83200,00</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>45435,00</t>
+          <t>41060,00</t>
         </is>
       </c>
       <c r="E12" s="3" t="n">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="F12" s="3" t="inlineStr">
         <is>
@@ -999,12 +999,12 @@
       </c>
       <c r="H12" s="3" t="inlineStr">
         <is>
-          <t>110 x R$ 843,00</t>
+          <t>147 x R$ 716,00</t>
         </is>
       </c>
       <c r="I12" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J12" s="3" t="inlineStr"/>
@@ -1022,20 +1022,20 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>94100,00</t>
+          <t>86000,00</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>26205,00</t>
+          <t>46800,00</t>
         </is>
       </c>
       <c r="E13" s="3" t="n">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="F13" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G13" s="3" t="inlineStr">
@@ -1045,20 +1045,15 @@
       </c>
       <c r="H13" s="3" t="inlineStr">
         <is>
-          <t>4 x R$ 1865,00
-73 x R$ 1489,00</t>
+          <t>111 x R$ 588,00</t>
         </is>
       </c>
       <c r="I13" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J13" s="3" t="inlineStr">
-        <is>
-          <t>sendo 4 x 1.865,00 + 73 x 1.489,00</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J13" s="3" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
@@ -1073,16 +1068,16 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>96200,00</t>
+          <t>92367,00</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>65810,00</t>
+          <t>26118,35</t>
         </is>
       </c>
       <c r="E14" s="3" t="n">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="F14" s="3" t="inlineStr">
         <is>
@@ -1091,20 +1086,25 @@
       </c>
       <c r="G14" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H14" s="3" t="inlineStr">
         <is>
-          <t>140 x R$ 410,00</t>
+          <t>3 x R$ 1865,00
+73 x R$ 1489,00</t>
         </is>
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J14" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>sendo 3 x 1.865,00 + 73 x 1.489,00</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
@@ -1119,20 +1119,20 @@
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>96700,00</t>
+          <t>96420,00</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>43335,00</t>
+          <t>23821,00</t>
         </is>
       </c>
       <c r="E15" s="3" t="n">
-        <v>152</v>
+        <v>61</v>
       </c>
       <c r="F15" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G15" s="3" t="inlineStr">
@@ -1142,15 +1142,20 @@
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>152 x R$ 637,00</t>
+          <t>3 x R$ 2491,00
+58 x R$ 1934,00</t>
         </is>
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J15" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J15" s="3" t="inlineStr">
+        <is>
+          <t>sendo 3 x 2.491,00 + 58 x 1.934,00</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
@@ -1165,16 +1170,16 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>97500,00</t>
+          <t>96700,00</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>47775,00</t>
+          <t>44035,00</t>
         </is>
       </c>
       <c r="E16" s="3" t="n">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
@@ -1183,17 +1188,17 @@
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H16" s="3" t="inlineStr">
         <is>
-          <t>147 x R$ 655,54</t>
+          <t>151 x R$ 637,00</t>
         </is>
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J16" s="3" t="inlineStr"/>
@@ -1211,16 +1216,16 @@
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>98600,00</t>
+          <t>98460,00</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>23930,00</t>
+          <t>53923,00</t>
         </is>
       </c>
       <c r="E17" s="3" t="n">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="F17" s="3" t="inlineStr">
         <is>
@@ -1234,20 +1239,15 @@
       </c>
       <c r="H17" s="3" t="inlineStr">
         <is>
-          <t>4 x R$ 2491,00
-58 x R$ 1934,00</t>
+          <t>109 x R$ 941,00</t>
         </is>
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J17" s="3" t="inlineStr">
-        <is>
-          <t>sendo 4 x 2.491,00 + 58 x 1.934,00</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J17" s="3" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
@@ -1262,16 +1262,16 @@
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>101100,00</t>
+          <t>99490,00</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>51655,00</t>
+          <t>52974,50</t>
         </is>
       </c>
       <c r="E18" s="3" t="n">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F18" s="3" t="inlineStr">
         <is>
@@ -1285,12 +1285,12 @@
       </c>
       <c r="H18" s="3" t="inlineStr">
         <is>
-          <t>192 x R$ 680,00</t>
+          <t>186 x R$ 554,00</t>
         </is>
       </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J18" s="3" t="inlineStr"/>
@@ -1308,20 +1308,20 @@
       </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t>102300,00</t>
+          <t>102420,00</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>53105,00</t>
+          <t>48021,00</t>
         </is>
       </c>
       <c r="E19" s="3" t="n">
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="F19" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G19" s="3" t="inlineStr">
@@ -1331,12 +1331,12 @@
       </c>
       <c r="H19" s="3" t="inlineStr">
         <is>
-          <t>130 x R$ 905,00</t>
+          <t>175 x R$ 711,00</t>
         </is>
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J19" s="3" t="inlineStr"/>
@@ -1359,11 +1359,11 @@
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>50200,00</t>
+          <t>50890,00</t>
         </is>
       </c>
       <c r="E20" s="3" t="n">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F20" s="3" t="inlineStr">
         <is>
@@ -1372,17 +1372,17 @@
       </c>
       <c r="G20" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H20" s="3" t="inlineStr">
         <is>
-          <t>184 x R$ 687,00</t>
+          <t>183 x R$ 687,00</t>
         </is>
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J20" s="3" t="inlineStr"/>
@@ -1400,20 +1400,20 @@
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>104400,00</t>
+          <t>105000,00</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>53220,00</t>
+          <t>50750,00</t>
         </is>
       </c>
       <c r="E21" s="3" t="n">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="F21" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G21" s="3" t="inlineStr">
@@ -1423,12 +1423,12 @@
       </c>
       <c r="H21" s="3" t="inlineStr">
         <is>
-          <t>130 x R$ 945,00</t>
+          <t>168 x R$ 695,00</t>
         </is>
       </c>
       <c r="I21" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J21" s="3" t="inlineStr"/>
@@ -1446,16 +1446,16 @@
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>105100,00</t>
+          <t>107000,00</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>46516,00</t>
+          <t>48350,00</t>
         </is>
       </c>
       <c r="E22" s="3" t="n">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="F22" s="3" t="inlineStr">
         <is>
@@ -1464,17 +1464,17 @@
       </c>
       <c r="G22" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H22" s="3" t="inlineStr">
         <is>
-          <t>175 x R$ 661,00</t>
+          <t>137 x R$ 929,00</t>
         </is>
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J22" s="3" t="inlineStr"/>
@@ -1492,16 +1492,16 @@
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>106400,00</t>
+          <t>108000,00</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>57310,00</t>
+          <t>58900,00</t>
         </is>
       </c>
       <c r="E23" s="3" t="n">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="F23" s="3" t="inlineStr">
         <is>
@@ -1515,12 +1515,12 @@
       </c>
       <c r="H23" s="3" t="inlineStr">
         <is>
-          <t>178 x R$ 653,00</t>
+          <t>188 x R$ 584,00</t>
         </is>
       </c>
       <c r="I23" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J23" s="3" t="inlineStr"/>
@@ -1538,16 +1538,16 @@
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>107000,00</t>
+          <t>111000,00</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>47350,00</t>
+          <t>55550,00</t>
         </is>
       </c>
       <c r="E24" s="3" t="n">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F24" s="3" t="inlineStr">
         <is>
@@ -1561,12 +1561,12 @@
       </c>
       <c r="H24" s="3" t="inlineStr">
         <is>
-          <t>138 x R$ 929,00</t>
+          <t>130 x R$ 924,00</t>
         </is>
       </c>
       <c r="I24" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J24" s="3" t="inlineStr"/>
@@ -1584,20 +1584,20 @@
       </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t>108000,00</t>
+          <t>112520,00</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>57900,00</t>
+          <t>54526,00</t>
         </is>
       </c>
       <c r="E25" s="3" t="n">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="F25" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G25" s="3" t="inlineStr">
@@ -1607,12 +1607,12 @@
       </c>
       <c r="H25" s="3" t="inlineStr">
         <is>
-          <t>189 x R$ 584,00</t>
+          <t>139 x R$ 794,00</t>
         </is>
       </c>
       <c r="I25" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J25" s="3" t="inlineStr"/>
@@ -1630,16 +1630,16 @@
       </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
-          <t>108500,00</t>
+          <t>112525,00</t>
         </is>
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>46125,00</t>
+          <t>54526,25</t>
         </is>
       </c>
       <c r="E26" s="3" t="n">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F26" s="3" t="inlineStr">
         <is>
@@ -1648,17 +1648,17 @@
       </c>
       <c r="G26" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H26" s="3" t="inlineStr">
         <is>
-          <t>172 x R$ 714,00</t>
+          <t>163 x R$ 791,00</t>
         </is>
       </c>
       <c r="I26" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J26" s="3" t="inlineStr"/>
@@ -1676,35 +1676,35 @@
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>109000,00</t>
+          <t>118700,00</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>69440,00</t>
+          <t>47935,00</t>
         </is>
       </c>
       <c r="E27" s="3" t="n">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="F27" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G27" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H27" s="3" t="inlineStr">
         <is>
-          <t>178 x R$ 553,00</t>
+          <t>196 x R$ 734,00</t>
         </is>
       </c>
       <c r="I27" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J27" s="3" t="inlineStr"/>
@@ -1722,20 +1722,20 @@
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>110000,00</t>
+          <t>124000,00</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>56490,00</t>
+          <t>61100,00</t>
         </is>
       </c>
       <c r="E28" s="3" t="n">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="F28" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G28" s="3" t="inlineStr">
@@ -1745,12 +1745,12 @@
       </c>
       <c r="H28" s="3" t="inlineStr">
         <is>
-          <t>134 x R$ 942,00</t>
+          <t>149 x R$ 825,00</t>
         </is>
       </c>
       <c r="I28" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J28" s="3" t="inlineStr"/>
@@ -1768,38 +1768,43 @@
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>110500,00</t>
+          <t>125790,00</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>54425,00</t>
+          <t>42289,50</t>
         </is>
       </c>
       <c r="E29" s="3" t="n">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="F29" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G29" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H29" s="3" t="inlineStr">
         <is>
-          <t>131 x R$ 924,00</t>
+          <t>3 x R$ 2613,70
+87 x R$ 1828,30</t>
         </is>
       </c>
       <c r="I29" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J29" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J29" s="3" t="inlineStr">
+        <is>
+          <t>sendo 3 x 2.613,70  + 87 x 1.828,30</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
@@ -1814,20 +1819,20 @@
       </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
-          <t>111900,00</t>
+          <t>129650,00</t>
         </is>
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>53595,00</t>
+          <t>76982,50</t>
         </is>
       </c>
       <c r="E30" s="3" t="n">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="F30" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G30" s="3" t="inlineStr">
@@ -1837,15 +1842,20 @@
       </c>
       <c r="H30" s="3" t="inlineStr">
         <is>
-          <t>140 x R$ 794,00</t>
+          <t>1 x R$ 1490,00
+95 x R$ 1187,00</t>
         </is>
       </c>
       <c r="I30" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J30" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J30" s="3" t="inlineStr">
+        <is>
+          <t>sendo 1 x 1.490,00 + 95 x 1.187,00</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
@@ -1860,16 +1870,16 @@
       </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>113300,00</t>
+          <t>134849,00</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>53965,00</t>
+          <t>48242,45</t>
         </is>
       </c>
       <c r="E31" s="3" t="n">
-        <v>157</v>
+        <v>86</v>
       </c>
       <c r="F31" s="3" t="inlineStr">
         <is>
@@ -1878,20 +1888,25 @@
       </c>
       <c r="G31" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H31" s="3" t="inlineStr">
         <is>
-          <t>157 x R$ 875,00</t>
+          <t>3 x R$ 2454,00
+83 x R$ 1672,00</t>
         </is>
       </c>
       <c r="I31" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J31" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J31" s="3" t="inlineStr">
+        <is>
+          <t>sendo 3 x 2.454,00 + 83 x 1.672,00</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
@@ -1906,20 +1921,20 @@
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>113400,00</t>
+          <t>135000,00</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>58660,00</t>
+          <t>73750,00</t>
         </is>
       </c>
       <c r="E32" s="3" t="n">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="F32" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G32" s="3" t="inlineStr">
@@ -1929,12 +1944,12 @@
       </c>
       <c r="H32" s="3" t="inlineStr">
         <is>
-          <t>157 x R$ 875,00</t>
+          <t>129 x R$ 892,00</t>
         </is>
       </c>
       <c r="I32" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J32" s="3" t="inlineStr"/>
@@ -1952,16 +1967,16 @@
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>113780,00</t>
+          <t>135000,00</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>58189,00</t>
+          <t>67750,00</t>
         </is>
       </c>
       <c r="E33" s="3" t="n">
-        <v>155</v>
+        <v>92</v>
       </c>
       <c r="F33" s="3" t="inlineStr">
         <is>
@@ -1975,12 +1990,12 @@
       </c>
       <c r="H33" s="3" t="inlineStr">
         <is>
-          <t>155 x R$ 796,00</t>
+          <t>92 x R$ 1395,00</t>
         </is>
       </c>
       <c r="I33" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J33" s="3" t="inlineStr"/>
@@ -1998,16 +2013,16 @@
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>116000,00</t>
+          <t>135300,00</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>65800,00</t>
+          <t>51215,00</t>
         </is>
       </c>
       <c r="E34" s="3" t="n">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="F34" s="3" t="inlineStr">
         <is>
@@ -2016,20 +2031,25 @@
       </c>
       <c r="G34" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H34" s="3" t="inlineStr">
         <is>
-          <t>117 x R$ 908,00</t>
+          <t>1 x R$ 2478,60
+87 x R$ 1693,00</t>
         </is>
       </c>
       <c r="I34" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J34" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J34" s="3" t="inlineStr">
+        <is>
+          <t>sendo 01 x 2.478,60 + 87 x 1.693,00</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
@@ -2044,16 +2064,16 @@
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>116480,00</t>
+          <t>135466,01</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>63824,00</t>
+          <t>43273,30</t>
         </is>
       </c>
       <c r="E35" s="3" t="n">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F35" s="3" t="inlineStr">
         <is>
@@ -2062,23 +2082,23 @@
       </c>
       <c r="G35" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H35" s="3" t="inlineStr">
         <is>
-          <t>2 x R$ 1650,00
-111 x R$ 967,00</t>
+          <t>3 x R$ 2467,00
+85 x R$ 1682,00</t>
         </is>
       </c>
       <c r="I35" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J35" s="3" t="inlineStr">
         <is>
-          <t>sendo 02 x 1650,00 + 111 x 967,00</t>
+          <t>sendo 3 x 2.467,00 + 85 x 1.682,00</t>
         </is>
       </c>
     </row>
@@ -2095,16 +2115,16 @@
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>117000,00</t>
+          <t>135472,00</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>62350,00</t>
+          <t>43673,60</t>
         </is>
       </c>
       <c r="E36" s="3" t="n">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F36" s="3" t="inlineStr">
         <is>
@@ -2113,23 +2133,23 @@
       </c>
       <c r="G36" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H36" s="3" t="inlineStr">
         <is>
-          <t>2 x R$ 1651,00
-111 x R$ 989,00</t>
+          <t>3 x R$ 2460,00
+85 x R$ 1676,00</t>
         </is>
       </c>
       <c r="I36" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J36" s="3" t="inlineStr">
         <is>
-          <t>sendo 02 x 1651,00 + 111 x 989,00</t>
+          <t>sendo 3 x 2.460,00 + 85 x 1.676,00</t>
         </is>
       </c>
     </row>
@@ -2146,20 +2166,20 @@
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>118700,00</t>
+          <t>136893,24</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
         <is>
-          <t>47935,00</t>
+          <t>43144,66</t>
         </is>
       </c>
       <c r="E37" s="3" t="n">
-        <v>196</v>
+        <v>67</v>
       </c>
       <c r="F37" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G37" s="3" t="inlineStr">
@@ -2169,15 +2189,20 @@
       </c>
       <c r="H37" s="3" t="inlineStr">
         <is>
-          <t>196 x R$ 734,00</t>
+          <t>2 x R$ 3252,00
+65 x R$ 2414,00</t>
         </is>
       </c>
       <c r="I37" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J37" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr">
+        <is>
+          <t>sendo 02 x 3.252,00 + 65 x 2.414,00</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
@@ -2192,20 +2217,20 @@
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>120000,00</t>
+          <t>137200,00</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
         <is>
-          <t>60000,00</t>
+          <t>78760,00</t>
         </is>
       </c>
       <c r="E38" s="3" t="n">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="F38" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G38" s="3" t="inlineStr">
@@ -2215,12 +2240,12 @@
       </c>
       <c r="H38" s="3" t="inlineStr">
         <is>
-          <t>101 x R$ 1099,00</t>
+          <t>141 x R$ 1099,00</t>
         </is>
       </c>
       <c r="I38" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J38" s="3" t="inlineStr"/>
@@ -2238,35 +2263,35 @@
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>121000,00</t>
+          <t>144060,00</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
         <is>
-          <t>56050,00</t>
+          <t>65503,00</t>
         </is>
       </c>
       <c r="E39" s="3" t="n">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="F39" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G39" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H39" s="3" t="inlineStr">
         <is>
-          <t>165 x R$ 804,00</t>
+          <t>186 x R$ 965,00</t>
         </is>
       </c>
       <c r="I39" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J39" s="3" t="inlineStr"/>
@@ -2284,16 +2309,16 @@
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>122120,00</t>
+          <t>144800,00</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
         <is>
-          <t>68106,00</t>
+          <t>41240,00</t>
         </is>
       </c>
       <c r="E40" s="3" t="n">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="F40" s="3" t="inlineStr">
         <is>
@@ -2307,15 +2332,20 @@
       </c>
       <c r="H40" s="3" t="inlineStr">
         <is>
-          <t>101 x R$ 1078,00</t>
+          <t>3 x R$ 3063,00
+71 x R$ 2236,00</t>
         </is>
       </c>
       <c r="I40" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J40" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>sendo 3 x 3.063,00 + 71 x 2.236,00</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="inlineStr">
@@ -2330,16 +2360,16 @@
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>123500,00</t>
+          <t>145000,00</t>
         </is>
       </c>
       <c r="D41" s="3" t="inlineStr">
         <is>
-          <t>60175,00</t>
+          <t>74650,00</t>
         </is>
       </c>
       <c r="E41" s="3" t="n">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="F41" s="3" t="inlineStr">
         <is>
@@ -2353,12 +2383,12 @@
       </c>
       <c r="H41" s="3" t="inlineStr">
         <is>
-          <t>151 x R$ 825,00</t>
+          <t>159 x R$ 1060,00</t>
         </is>
       </c>
       <c r="I41" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J41" s="3" t="inlineStr"/>
@@ -2376,20 +2406,20 @@
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>127800,00</t>
+          <t>148020,00</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
         <is>
-          <t>42390,00</t>
+          <t>72901,00</t>
         </is>
       </c>
       <c r="E42" s="3" t="n">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F42" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G42" s="3" t="inlineStr">
@@ -2399,20 +2429,15 @@
       </c>
       <c r="H42" s="3" t="inlineStr">
         <is>
-          <t>4 x R$ 2613,70
-87 x R$ 1828,30</t>
+          <t>61 x R$ 2021,00</t>
         </is>
       </c>
       <c r="I42" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J42" s="3" t="inlineStr">
-        <is>
-          <t>sendo 4 x 2.613,70  + 87 x 1.828,30</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
@@ -2427,20 +2452,20 @@
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>133000,00</t>
+          <t>151180,00</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>65950,00</t>
+          <t>71559,00</t>
         </is>
       </c>
       <c r="E43" s="3" t="n">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="F43" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G43" s="3" t="inlineStr">
@@ -2450,12 +2475,12 @@
       </c>
       <c r="H43" s="3" t="inlineStr">
         <is>
-          <t>94 x R$ 1400,00</t>
+          <t>142 x R$ 1114,00</t>
         </is>
       </c>
       <c r="I43" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J43" s="3" t="inlineStr"/>
@@ -2473,16 +2498,16 @@
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>135300,00</t>
+          <t>154000,00</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>48765,00</t>
+          <t>83700,00</t>
         </is>
       </c>
       <c r="E44" s="3" t="n">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
@@ -2496,20 +2521,15 @@
       </c>
       <c r="H44" s="3" t="inlineStr">
         <is>
-          <t>2 x R$ 2478,60
-87 x R$ 1693,00</t>
+          <t>169 x R$ 995,00</t>
         </is>
       </c>
       <c r="I44" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J44" s="3" t="inlineStr">
-        <is>
-          <t>sendo 02 x 2.478,60 + 87 x 1.693,00</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
@@ -2524,20 +2544,20 @@
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>136000,00</t>
+          <t>156000,00</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
         <is>
-          <t>65700,00</t>
+          <t>86800,00</t>
         </is>
       </c>
       <c r="E45" s="3" t="n">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G45" s="3" t="inlineStr">
@@ -2547,12 +2567,12 @@
       </c>
       <c r="H45" s="3" t="inlineStr">
         <is>
-          <t>156 x R$ 1089,00</t>
+          <t>115 x R$ 1022,00</t>
         </is>
       </c>
       <c r="I45" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J45" s="3" t="inlineStr"/>
@@ -2570,43 +2590,38 @@
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>136893,24</t>
+          <t>156000,00</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
         <is>
-          <t>39844,66</t>
+          <t>86800,00</t>
         </is>
       </c>
       <c r="E46" s="3" t="n">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="F46" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G46" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H46" s="3" t="inlineStr">
         <is>
-          <t>3 x R$ 3252,00
-65 x R$ 2414,00</t>
+          <t>115 x R$ 1022,00</t>
         </is>
       </c>
       <c r="I46" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J46" s="3" t="inlineStr">
-        <is>
-          <t>sendo 03 x 3.252,00 + 65 x 2.414,00</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
@@ -2621,20 +2636,20 @@
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>136900,00</t>
+          <t>156000,00</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
         <is>
-          <t>48345,00</t>
+          <t>86800,00</t>
         </is>
       </c>
       <c r="E47" s="3" t="n">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="F47" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G47" s="3" t="inlineStr">
@@ -2644,20 +2659,15 @@
       </c>
       <c r="H47" s="3" t="inlineStr">
         <is>
-          <t>4 x R$ 2454,00
-83 x R$ 1672,00</t>
+          <t>115 x R$ 1022,00</t>
         </is>
       </c>
       <c r="I47" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J47" s="3" t="inlineStr">
-        <is>
-          <t>sendo 4 x 2.454,00 + 83 x 1.672,00</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J47" s="3" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
@@ -2672,43 +2682,38 @@
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>137500,00</t>
+          <t>161000,00</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>43375,00</t>
+          <t>77950,00</t>
         </is>
       </c>
       <c r="E48" s="3" t="n">
-        <v>89</v>
+        <v>142</v>
       </c>
       <c r="F48" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G48" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H48" s="3" t="inlineStr">
         <is>
-          <t>4 x R$ 2467,00
-85 x R$ 1682,00</t>
+          <t>142 x R$ 1115,00</t>
         </is>
       </c>
       <c r="I48" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J48" s="3" t="inlineStr">
-        <is>
-          <t>sendo 4 x 2.467,00 + 85 x 1.682,00</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
@@ -2723,20 +2728,20 @@
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>137500,00</t>
+          <t>194250,00</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>43775,00</t>
+          <t>104712,50</t>
         </is>
       </c>
       <c r="E49" s="3" t="n">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="F49" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G49" s="3" t="inlineStr">
@@ -2746,18 +2751,18 @@
       </c>
       <c r="H49" s="3" t="inlineStr">
         <is>
-          <t>4 x R$ 2460,00
-85 x R$ 1676,00</t>
+          <t>129 x R$ 1342,00
+21 x R$ 450,00</t>
         </is>
       </c>
       <c r="I49" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J49" s="3" t="inlineStr">
         <is>
-          <t>sendo 4 x 2.460,00 + 85 x 1.676,00</t>
+          <t>sendo 129 x 1.342,00 + 21 x 450,00</t>
         </is>
       </c>
     </row>
@@ -2774,20 +2779,20 @@
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>144000,00</t>
+          <t>200000,00</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
         <is>
-          <t>73200,00</t>
+          <t>100000,00</t>
         </is>
       </c>
       <c r="E50" s="3" t="n">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="F50" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G50" s="3" t="inlineStr">
@@ -2797,12 +2802,12 @@
       </c>
       <c r="H50" s="3" t="inlineStr">
         <is>
-          <t>160 x R$ 1060,00</t>
+          <t>193 x R$ 1253,00</t>
         </is>
       </c>
       <c r="I50" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J50" s="3" t="inlineStr"/>
@@ -2820,20 +2825,20 @@
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>150000,00</t>
+          <t>200900,00</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>76300,00</t>
+          <t>100945,00</t>
         </is>
       </c>
       <c r="E51" s="3" t="n">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="F51" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Sicoob</t>
         </is>
       </c>
       <c r="G51" s="3" t="inlineStr">
@@ -2843,12 +2848,12 @@
       </c>
       <c r="H51" s="3" t="inlineStr">
         <is>
-          <t>85 x R$ 1850,00</t>
+          <t>135 x R$ 1235,00</t>
         </is>
       </c>
       <c r="I51" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J51" s="3" t="inlineStr"/>
@@ -2866,16 +2871,16 @@
       </c>
       <c r="C52" s="3" t="inlineStr">
         <is>
-          <t>153000,00</t>
+          <t>205000,00</t>
         </is>
       </c>
       <c r="D52" s="3" t="inlineStr">
         <is>
-          <t>83650,00</t>
+          <t>101150,00</t>
         </is>
       </c>
       <c r="E52" s="3" t="n">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="F52" s="3" t="inlineStr">
         <is>
@@ -2889,12 +2894,12 @@
       </c>
       <c r="H52" s="3" t="inlineStr">
         <is>
-          <t>170 x R$ 995,00</t>
+          <t>193 x R$ 1234,00</t>
         </is>
       </c>
       <c r="I52" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J52" s="3" t="inlineStr"/>
@@ -2912,20 +2917,20 @@
       </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>169000,00</t>
+          <t>208050,00</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>80450,00</t>
+          <t>108902,50</t>
         </is>
       </c>
       <c r="E53" s="3" t="n">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="F53" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G53" s="3" t="inlineStr">
@@ -2935,12 +2940,12 @@
       </c>
       <c r="H53" s="3" t="inlineStr">
         <is>
-          <t>147 x R$ 1074,00</t>
+          <t>178 x R$ 1417,00</t>
         </is>
       </c>
       <c r="I53" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J53" s="3" t="inlineStr"/>
@@ -2958,20 +2963,20 @@
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>171000,00</t>
+          <t>212000,00</t>
         </is>
       </c>
       <c r="D54" s="3" t="inlineStr">
         <is>
-          <t>73550,00</t>
+          <t>101500,00</t>
         </is>
       </c>
       <c r="E54" s="3" t="n">
-        <v>56</v>
+        <v>136</v>
       </c>
       <c r="F54" s="3" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G54" s="3" t="inlineStr">
@@ -2981,12 +2986,12 @@
       </c>
       <c r="H54" s="3" t="inlineStr">
         <is>
-          <t>56 x R$ 3548,92</t>
+          <t>136 x R$ 1759,00</t>
         </is>
       </c>
       <c r="I54" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J54" s="3" t="inlineStr"/>
@@ -3004,38 +3009,43 @@
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>187600,00</t>
+          <t>225050,00</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
         <is>
-          <t>93380,00</t>
+          <t>109052,50</t>
         </is>
       </c>
       <c r="E55" s="3" t="n">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="F55" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G55" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H55" s="3" t="inlineStr">
         <is>
-          <t>154 x R$ 1054,60</t>
+          <t>139 x R$ 1585,00
+24 x R$ 791,00</t>
         </is>
       </c>
       <c r="I55" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J55" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr">
+        <is>
+          <t>sendo 139 x 1.585,00 + 24 x 791,00</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
@@ -3050,20 +3060,20 @@
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>208000,00</t>
+          <t>236600,00</t>
         </is>
       </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>108900,00</t>
+          <t>131830,00</t>
         </is>
       </c>
       <c r="E56" s="3" t="n">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="F56" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G56" s="3" t="inlineStr">
@@ -3073,12 +3083,12 @@
       </c>
       <c r="H56" s="3" t="inlineStr">
         <is>
-          <t>177 x R$ 1417,00</t>
+          <t>81 x R$ 1727,00</t>
         </is>
       </c>
       <c r="I56" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J56" s="3" t="inlineStr"/>
@@ -3096,35 +3106,35 @@
       </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t>209496,00</t>
+          <t>257500,00</t>
         </is>
       </c>
       <c r="D57" s="3" t="inlineStr">
         <is>
-          <t>95074,80</t>
+          <t>125775,00</t>
         </is>
       </c>
       <c r="E57" s="3" t="n">
-        <v>157</v>
+        <v>101</v>
       </c>
       <c r="F57" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G57" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H57" s="3" t="inlineStr">
         <is>
-          <t>157 x R$ 1553,00</t>
+          <t>101 x R$ 2303,00</t>
         </is>
       </c>
       <c r="I57" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J57" s="3" t="inlineStr"/>
@@ -3142,38 +3152,45 @@
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>218063,00</t>
+          <t>274394,00</t>
         </is>
       </c>
       <c r="D58" s="3" t="inlineStr">
         <is>
-          <t>100803,15</t>
+          <t>83219,70</t>
         </is>
       </c>
       <c r="E58" s="3" t="n">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="F58" s="3" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G58" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H58" s="3" t="inlineStr">
         <is>
-          <t>120 x R$ 2125,00</t>
+          <t>3 x R$ 5719,00
+1 x R$ 4881,00
+64 x R$ 4096,00
+20 x R$ 1682,00</t>
         </is>
       </c>
       <c r="I58" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J58" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr">
+        <is>
+          <t>sendo 3 x 5.719,00 + 1 x 4.881,00 + 64 x 4.096,00 + 20 x 1.682,00</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
@@ -3188,43 +3205,38 @@
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>229500,00</t>
+          <t>300000,00</t>
         </is>
       </c>
       <c r="D59" s="3" t="inlineStr">
         <is>
-          <t>101475,00</t>
+          <t>172000,00</t>
         </is>
       </c>
       <c r="E59" s="3" t="n">
-        <v>173</v>
+        <v>97</v>
       </c>
       <c r="F59" s="3" t="inlineStr">
         <is>
-          <t>Bradesco</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G59" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H59" s="3" t="inlineStr">
         <is>
-          <t>165 x R$ 1518,00
-8 x R$ 714,00</t>
+          <t>97 x R$ 2568,00</t>
         </is>
       </c>
       <c r="I59" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J59" s="3" t="inlineStr">
-        <is>
-          <t>sendo 165 x 1518,00 + 08 x 714,00</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
@@ -3239,43 +3251,38 @@
       </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>236100,00</t>
+          <t>364000,00</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
         <is>
-          <t>67305,00</t>
+          <t>273100,00</t>
         </is>
       </c>
       <c r="E60" s="3" t="n">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="F60" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G60" s="3" t="inlineStr">
         <is>
-          <t>Indisponível</t>
+          <t>Disponível</t>
         </is>
       </c>
       <c r="H60" s="3" t="inlineStr">
         <is>
-          <t>4 x R$ 4958,00
-58 x R$ 3616,00</t>
+          <t>27 x R$ 4498,00</t>
         </is>
       </c>
       <c r="I60" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J60" s="3" t="inlineStr">
-        <is>
-          <t>sendo 4 x 4.958,00 + 58 x 3.616,00 + 1.682,00</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
@@ -3290,20 +3297,20 @@
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>243500,00</t>
+          <t>367000,00</t>
         </is>
       </c>
       <c r="D61" s="3" t="inlineStr">
         <is>
-          <t>140175,00</t>
+          <t>246250,00</t>
         </is>
       </c>
       <c r="E61" s="3" t="n">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="F61" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Santander</t>
         </is>
       </c>
       <c r="G61" s="3" t="inlineStr">
@@ -3313,12 +3320,12 @@
       </c>
       <c r="H61" s="3" t="inlineStr">
         <is>
-          <t>154 x R$ 1406,00</t>
+          <t>85 x R$ 2191,00</t>
         </is>
       </c>
       <c r="I61" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J61" s="3" t="inlineStr"/>
@@ -3336,16 +3343,16 @@
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>300000,00</t>
+          <t>475050,00</t>
         </is>
       </c>
       <c r="D62" s="3" t="inlineStr">
         <is>
-          <t>172000,00</t>
+          <t>253252,50</t>
         </is>
       </c>
       <c r="E62" s="3" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F62" s="3" t="inlineStr">
         <is>
@@ -3359,12 +3366,12 @@
       </c>
       <c r="H62" s="3" t="inlineStr">
         <is>
-          <t>98 x R$ 2568,00</t>
+          <t>106 x R$ 3603,00</t>
         </is>
       </c>
       <c r="I62" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J62" s="3" t="inlineStr"/>
@@ -3382,16 +3389,16 @@
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>300000,00</t>
+          <t>500000,00</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
         <is>
-          <t>172000,00</t>
+          <t>268000,00</t>
         </is>
       </c>
       <c r="E63" s="3" t="n">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="F63" s="3" t="inlineStr">
         <is>
@@ -3405,12 +3412,12 @@
       </c>
       <c r="H63" s="3" t="inlineStr">
         <is>
-          <t>98 x R$ 2568,00</t>
+          <t>189 x R$ 3100,00</t>
         </is>
       </c>
       <c r="I63" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J63" s="3" t="inlineStr"/>
@@ -3428,20 +3435,20 @@
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>331300,00</t>
+          <t>587600,00</t>
         </is>
       </c>
       <c r="D64" s="3" t="inlineStr">
         <is>
-          <t>166465,00</t>
+          <t>283380,00</t>
         </is>
       </c>
       <c r="E64" s="3" t="n">
-        <v>234</v>
+        <v>109</v>
       </c>
       <c r="F64" s="3" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G64" s="3" t="inlineStr">
@@ -3451,12 +3458,12 @@
       </c>
       <c r="H64" s="3" t="inlineStr">
         <is>
-          <t>234 x R$ 1699,00</t>
+          <t>109 x R$ 4758,00</t>
         </is>
       </c>
       <c r="I64" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J64" s="3" t="inlineStr"/>
@@ -3474,20 +3481,20 @@
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>361400,00</t>
+          <t>711000,00</t>
         </is>
       </c>
       <c r="D65" s="3" t="inlineStr">
         <is>
-          <t>242070,00</t>
+          <t>377550,00</t>
         </is>
       </c>
       <c r="E65" s="3" t="n">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="F65" s="3" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G65" s="3" t="inlineStr">
@@ -3497,12 +3504,12 @@
       </c>
       <c r="H65" s="3" t="inlineStr">
         <is>
-          <t>87 x R$ 2191,00</t>
+          <t>112 x R$ 5736,00</t>
         </is>
       </c>
       <c r="I65" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J65" s="3" t="inlineStr"/>
@@ -3520,16 +3527,16 @@
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>377260,00</t>
+          <t>790000,00</t>
         </is>
       </c>
       <c r="D66" s="3" t="inlineStr">
         <is>
-          <t>194863,00</t>
+          <t>380400,00</t>
         </is>
       </c>
       <c r="E66" s="3" t="n">
-        <v>177</v>
+        <v>144</v>
       </c>
       <c r="F66" s="3" t="inlineStr">
         <is>
@@ -3543,12 +3550,12 @@
       </c>
       <c r="H66" s="3" t="inlineStr">
         <is>
-          <t>177 x R$ 2325,76</t>
+          <t>144 x R$ 6342,00</t>
         </is>
       </c>
       <c r="I66" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J66" s="3" t="inlineStr"/>
@@ -3566,16 +3573,16 @@
       </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
-          <t>385500,00</t>
+          <t>807000,00</t>
         </is>
       </c>
       <c r="D67" s="3" t="inlineStr">
         <is>
-          <t>248875,00</t>
+          <t>415350,00</t>
         </is>
       </c>
       <c r="E67" s="3" t="n">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="F67" s="3" t="inlineStr">
         <is>
@@ -3589,12 +3596,12 @@
       </c>
       <c r="H67" s="3" t="inlineStr">
         <is>
-          <t>155 x R$ 1805,00</t>
+          <t>112 x R$ 5876,00</t>
         </is>
       </c>
       <c r="I67" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J67" s="3" t="inlineStr"/>
@@ -3612,16 +3619,16 @@
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>402200,00</t>
+          <t>807000,00</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
         <is>
-          <t>134510,00</t>
+          <t>412350,00</t>
         </is>
       </c>
       <c r="E68" s="3" t="n">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="F68" s="3" t="inlineStr">
         <is>
@@ -3635,23 +3642,15 @@
       </c>
       <c r="H68" s="3" t="inlineStr">
         <is>
-          <t>4 x R$ 7527,70
-83 x R$ 5176,30
-2 x R$ 3504,30
-2 x R$ 1828,30</t>
+          <t>112 x R$ 5680,00</t>
         </is>
       </c>
       <c r="I68" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J68" s="3" t="inlineStr">
-        <is>
-          <t>sendo  4x 7.527,70 + 83 x 5.176,30 + 2 x 3.504,30 + 2 x 1.828,30
-junção</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J68" s="3" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
@@ -3661,25 +3660,25 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
         <is>
-          <t>404594,55</t>
+          <t>16600,00</t>
         </is>
       </c>
       <c r="D69" s="3" t="inlineStr">
         <is>
-          <t>216529,73</t>
+          <t>7330,00</t>
         </is>
       </c>
       <c r="E69" s="3" t="n">
-        <v>192</v>
+        <v>51</v>
       </c>
       <c r="F69" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G69" s="3" t="inlineStr">
@@ -3689,12 +3688,12 @@
       </c>
       <c r="H69" s="3" t="inlineStr">
         <is>
-          <t>192 x R$ 2611,00</t>
+          <t>51 x R$ 320,00</t>
         </is>
       </c>
       <c r="I69" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J69" s="3" t="inlineStr"/>
@@ -3707,25 +3706,25 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
         <is>
-          <t>426000,00</t>
+          <t>28700,00</t>
         </is>
       </c>
       <c r="D70" s="3" t="inlineStr">
         <is>
-          <t>210000,00</t>
+          <t>18535,00</t>
         </is>
       </c>
       <c r="E70" s="3" t="n">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="F70" s="3" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G70" s="3" t="inlineStr">
@@ -3735,12 +3734,12 @@
       </c>
       <c r="H70" s="3" t="inlineStr">
         <is>
-          <t>126 x R$ 3108,00</t>
+          <t>70 x R$ 226,74</t>
         </is>
       </c>
       <c r="I70" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J70" s="3" t="inlineStr"/>
@@ -3753,21 +3752,21 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t>434000,00</t>
+          <t>41400,00</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
         <is>
-          <t>220700,00</t>
+          <t>21570,00</t>
         </is>
       </c>
       <c r="E71" s="3" t="n">
-        <v>154</v>
+        <v>21</v>
       </c>
       <c r="F71" s="3" t="inlineStr">
         <is>
@@ -3781,21 +3780,15 @@
       </c>
       <c r="H71" s="3" t="inlineStr">
         <is>
-          <t>136 x R$ 3367,49
-18 x R$ 435,00</t>
+          <t>21 x R$ 1950,00</t>
         </is>
       </c>
       <c r="I71" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J71" s="3" t="inlineStr">
-        <is>
-          <t>sendo 136 x 3367,49 + 18 x 435,00
-JUNÇÃO</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J71" s="3" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
@@ -3805,25 +3798,25 @@
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
         <is>
-          <t>434250,00</t>
+          <t>41600,00</t>
         </is>
       </c>
       <c r="D72" s="3" t="inlineStr">
         <is>
-          <t>202712,50</t>
+          <t>20980,00</t>
         </is>
       </c>
       <c r="E72" s="3" t="n">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="F72" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Bradesco</t>
         </is>
       </c>
       <c r="G72" s="3" t="inlineStr">
@@ -3833,12 +3826,12 @@
       </c>
       <c r="H72" s="3" t="inlineStr">
         <is>
-          <t>2 x R$ 1376,00</t>
+          <t>69 x R$ 583,00</t>
         </is>
       </c>
       <c r="I72" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J72" s="3" t="inlineStr"/>
@@ -3851,21 +3844,21 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t>436000,00</t>
+          <t>44300,00</t>
         </is>
       </c>
       <c r="D73" s="3" t="inlineStr">
         <is>
-          <t>211800,00</t>
+          <t>20015,00</t>
         </is>
       </c>
       <c r="E73" s="3" t="n">
-        <v>178</v>
+        <v>40</v>
       </c>
       <c r="F73" s="3" t="inlineStr">
         <is>
@@ -3879,22 +3872,15 @@
       </c>
       <c r="H73" s="3" t="inlineStr">
         <is>
-          <t>21 x R$ 2974,89
-129 x R$ 2914,19
-28 x R$ 293,00</t>
+          <t>40 x R$ 911,00</t>
         </is>
       </c>
       <c r="I73" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J73" s="3" t="inlineStr">
-        <is>
-          <t>sendo 21 x 2974,89 + 129 x 2914,19 + 28 x 293,00
-JUNÇÃO</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J73" s="3" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
@@ -3904,25 +3890,25 @@
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>448000,00</t>
+          <t>52450,00</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
         <is>
-          <t>234800,00</t>
+          <t>19422,50</t>
         </is>
       </c>
       <c r="E74" s="3" t="n">
-        <v>208</v>
+        <v>44</v>
       </c>
       <c r="F74" s="3" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G74" s="3" t="inlineStr">
@@ -3932,12 +3918,12 @@
       </c>
       <c r="H74" s="3" t="inlineStr">
         <is>
-          <t>208 x R$ 2387,00</t>
+          <t>44 x R$ 1179,00</t>
         </is>
       </c>
       <c r="I74" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J74" s="3" t="inlineStr"/>
@@ -3950,21 +3936,21 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>459400,00</t>
+          <t>52700,00</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
         <is>
-          <t>222870,00</t>
+          <t>19535,00</t>
         </is>
       </c>
       <c r="E75" s="3" t="n">
-        <v>136</v>
+        <v>41</v>
       </c>
       <c r="F75" s="3" t="inlineStr">
         <is>
@@ -3978,21 +3964,15 @@
       </c>
       <c r="H75" s="3" t="inlineStr">
         <is>
-          <t>130 x R$ 3877,49
-6 x R$ 2932,49</t>
+          <t>41 x R$ 1250,00</t>
         </is>
       </c>
       <c r="I75" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J75" s="3" t="inlineStr">
-        <is>
-          <t>sendo 130 x 3877,49 + 06 x 2932,49
-JUNÇÃO</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J75" s="3" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
@@ -4002,21 +3982,21 @@
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>504273,00</t>
+          <t>53200,00</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
         <is>
-          <t>255213,65</t>
+          <t>17960,00</t>
         </is>
       </c>
       <c r="E76" s="3" t="n">
-        <v>138</v>
+        <v>41</v>
       </c>
       <c r="F76" s="3" t="inlineStr">
         <is>
@@ -4030,12 +4010,12 @@
       </c>
       <c r="H76" s="3" t="inlineStr">
         <is>
-          <t>138 x R$ 4242,00</t>
+          <t>41 x R$ 1322,00</t>
         </is>
       </c>
       <c r="I76" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J76" s="3" t="inlineStr"/>
@@ -4048,21 +4028,21 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
-          <t>522000,00</t>
+          <t>59880,00</t>
         </is>
       </c>
       <c r="D77" s="3" t="inlineStr">
         <is>
-          <t>267100,00</t>
+          <t>27094,00</t>
         </is>
       </c>
       <c r="E77" s="3" t="n">
-        <v>181</v>
+        <v>32</v>
       </c>
       <c r="F77" s="3" t="inlineStr">
         <is>
@@ -4076,12 +4056,12 @@
       </c>
       <c r="H77" s="3" t="inlineStr">
         <is>
-          <t>181 x R$ 3239,00</t>
+          <t>32 x R$ 1716,00</t>
         </is>
       </c>
       <c r="I77" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J77" s="3" t="inlineStr"/>
@@ -4094,25 +4074,25 @@
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t>531000,00</t>
+          <t>97500,00</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
         <is>
-          <t>273550,00</t>
+          <t>28875,00</t>
         </is>
       </c>
       <c r="E78" s="3" t="n">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="F78" s="3" t="inlineStr">
         <is>
-          <t>Santander</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G78" s="3" t="inlineStr">
@@ -4122,12 +4102,12 @@
       </c>
       <c r="H78" s="3" t="inlineStr">
         <is>
-          <t>95 x R$ 4560,00</t>
+          <t>35 x R$ 3053,00</t>
         </is>
       </c>
       <c r="I78" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J78" s="3" t="inlineStr"/>
@@ -4140,21 +4120,21 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
-          <t>539000,00</t>
+          <t>102440,00</t>
         </is>
       </c>
       <c r="D79" s="3" t="inlineStr">
         <is>
-          <t>275950,00</t>
+          <t>41622,00</t>
         </is>
       </c>
       <c r="E79" s="3" t="n">
-        <v>146</v>
+        <v>34</v>
       </c>
       <c r="F79" s="3" t="inlineStr">
         <is>
@@ -4163,17 +4143,17 @@
       </c>
       <c r="G79" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H79" s="3" t="inlineStr">
         <is>
-          <t>146 x R$ 4370,00</t>
+          <t>34 x R$ 2623,00</t>
         </is>
       </c>
       <c r="I79" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J79" s="3" t="inlineStr"/>
@@ -4186,25 +4166,25 @@
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
-          <t>539000,00</t>
+          <t>119000,00</t>
         </is>
       </c>
       <c r="D80" s="3" t="inlineStr">
         <is>
-          <t>282450,00</t>
+          <t>49150,00</t>
         </is>
       </c>
       <c r="E80" s="3" t="n">
-        <v>146</v>
+        <v>54</v>
       </c>
       <c r="F80" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G80" s="3" t="inlineStr">
@@ -4214,12 +4194,12 @@
       </c>
       <c r="H80" s="3" t="inlineStr">
         <is>
-          <t>146 x R$ 3679,00</t>
+          <t>54 x R$ 2620,00</t>
         </is>
       </c>
       <c r="I80" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J80" s="3" t="inlineStr"/>
@@ -4232,21 +4212,21 @@
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
         <is>
-          <t>550900,00</t>
+          <t>125200,00</t>
         </is>
       </c>
       <c r="D81" s="3" t="inlineStr">
         <is>
-          <t>221545,00</t>
+          <t>62260,00</t>
         </is>
       </c>
       <c r="E81" s="3" t="n">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="F81" s="3" t="inlineStr">
         <is>
@@ -4260,19 +4240,17 @@
       </c>
       <c r="H81" s="3" t="inlineStr">
         <is>
-          <t>29 x R$ 9925,49
-107 x R$ 2932,49</t>
+          <t>64 x R$ 1875,00</t>
         </is>
       </c>
       <c r="I81" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J81" s="3" t="inlineStr">
         <is>
-          <t>sendo 29 x 9925,49 + 107 x 2932,49
-JUNÇÃO</t>
+          <t>VP06</t>
         </is>
       </c>
     </row>
@@ -4284,25 +4262,25 @@
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
-          <t>609771,00</t>
+          <t>126000,00</t>
         </is>
       </c>
       <c r="D82" s="3" t="inlineStr">
         <is>
-          <t>292488,55</t>
+          <t>56955,00</t>
         </is>
       </c>
       <c r="E82" s="3" t="n">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="F82" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G82" s="3" t="inlineStr">
@@ -4312,19 +4290,15 @@
       </c>
       <c r="H82" s="3" t="inlineStr">
         <is>
-          <t>3 x R$ 6082,00</t>
+          <t>54 x R$ 2655,00</t>
         </is>
       </c>
       <c r="I82" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J82" s="3" t="inlineStr">
-        <is>
-          <t>Junção</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J82" s="3" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
@@ -4334,25 +4308,25 @@
       </c>
       <c r="B83" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>710000,00</t>
+          <t>132000,00</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
         <is>
-          <t>386800,00</t>
+          <t>63050,00</t>
         </is>
       </c>
       <c r="E83" s="3" t="n">
-        <v>145</v>
+        <v>53</v>
       </c>
       <c r="F83" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G83" s="3" t="inlineStr">
@@ -4362,12 +4336,12 @@
       </c>
       <c r="H83" s="3" t="inlineStr">
         <is>
-          <t>145 x R$ 4630,00</t>
+          <t>53 x R$ 2455,00</t>
         </is>
       </c>
       <c r="I83" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J83" s="3" t="inlineStr"/>
@@ -4380,21 +4354,21 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
         <is>
-          <t>710000,00</t>
+          <t>132500,00</t>
         </is>
       </c>
       <c r="D84" s="3" t="inlineStr">
         <is>
-          <t>377500,00</t>
+          <t>68625,00</t>
         </is>
       </c>
       <c r="E84" s="3" t="n">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="F84" s="3" t="inlineStr">
         <is>
@@ -4408,15 +4382,19 @@
       </c>
       <c r="H84" s="3" t="inlineStr">
         <is>
-          <t>113 x R$ 5736,00</t>
+          <t>67 x R$ 1803,00</t>
         </is>
       </c>
       <c r="I84" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J84" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J84" s="3" t="inlineStr">
+        <is>
+          <t>VP08</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
@@ -4426,25 +4404,25 @@
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t>770100,00</t>
+          <t>140000,00</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>410405,00</t>
+          <t>60200,00</t>
         </is>
       </c>
       <c r="E85" s="3" t="n">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="F85" s="3" t="inlineStr">
         <is>
-          <t>Porto Seguro</t>
+          <t>Itaú</t>
         </is>
       </c>
       <c r="G85" s="3" t="inlineStr">
@@ -4454,12 +4432,12 @@
       </c>
       <c r="H85" s="3" t="inlineStr">
         <is>
-          <t>109 x R$ 7675,00</t>
+          <t>41 x R$ 3678,00</t>
         </is>
       </c>
       <c r="I85" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J85" s="3" t="inlineStr"/>
@@ -4472,21 +4450,21 @@
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t>790000,00</t>
+          <t>153000,00</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>383500,00</t>
+          <t>78650,00</t>
         </is>
       </c>
       <c r="E86" s="3" t="n">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="F86" s="3" t="inlineStr">
         <is>
@@ -4500,12 +4478,12 @@
       </c>
       <c r="H86" s="3" t="inlineStr">
         <is>
-          <t>145 x R$ 6341,00</t>
+          <t>83 x R$ 1845,00</t>
         </is>
       </c>
       <c r="I86" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J86" s="3" t="inlineStr"/>
@@ -4518,21 +4496,21 @@
       </c>
       <c r="B87" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
-          <t>860000,00</t>
+          <t>158350,00</t>
         </is>
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>448800,00</t>
+          <t>56917,50</t>
         </is>
       </c>
       <c r="E87" s="3" t="n">
-        <v>168</v>
+        <v>44</v>
       </c>
       <c r="F87" s="3" t="inlineStr">
         <is>
@@ -4546,15 +4524,20 @@
       </c>
       <c r="H87" s="3" t="inlineStr">
         <is>
-          <t>168 x R$ 5368,00</t>
+          <t>41 x R$ 3751,00
+3 x R$ 1179,00</t>
         </is>
       </c>
       <c r="I87" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J87" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J87" s="3" t="inlineStr">
+        <is>
+          <t>sendo 41 x 3.751,00 + 3 x 1.179,00</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
@@ -4564,21 +4547,21 @@
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
         <is>
-          <t>1027000,00</t>
+          <t>200000,00</t>
         </is>
       </c>
       <c r="D88" s="3" t="inlineStr">
         <is>
-          <t>536350,00</t>
+          <t>89700,00</t>
         </is>
       </c>
       <c r="E88" s="3" t="n">
-        <v>194</v>
+        <v>114</v>
       </c>
       <c r="F88" s="3" t="inlineStr">
         <is>
@@ -4592,20 +4575,15 @@
       </c>
       <c r="H88" s="3" t="inlineStr">
         <is>
-          <t>181 x R$ 6489,00
-13 x R$ 3250,00</t>
+          <t>114 x R$ 2073,00</t>
         </is>
       </c>
       <c r="I88" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J88" s="3" t="inlineStr">
-        <is>
-          <t>Sendo  181 x 6.489,00 + 13 x 3.250,00  Junção</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J88" s="3" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
@@ -4615,21 +4593,21 @@
       </c>
       <c r="B89" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t>1065000,00</t>
+          <t>201050,00</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
         <is>
-          <t>558250,00</t>
+          <t>98052,50</t>
         </is>
       </c>
       <c r="E89" s="3" t="n">
-        <v>145</v>
+        <v>66</v>
       </c>
       <c r="F89" s="3" t="inlineStr">
         <is>
@@ -4643,21 +4621,15 @@
       </c>
       <c r="H89" s="3" t="inlineStr">
         <is>
-          <t>136 x R$ 7542,19
-9 x R$ 4609,70</t>
+          <t>66 x R$ 2903,00</t>
         </is>
       </c>
       <c r="I89" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J89" s="3" t="inlineStr">
-        <is>
-          <t>sendo 136 x 7542,19 + 09 x 4609,70
-JUNÇÃO</t>
-        </is>
-      </c>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J89" s="3" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
@@ -4667,21 +4639,21 @@
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Imóveis</t>
+          <t>Veículos</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
         <is>
-          <t>1090000,00</t>
+          <t>207550,00</t>
         </is>
       </c>
       <c r="D90" s="3" t="inlineStr">
         <is>
-          <t>555200,00</t>
+          <t>99377,50</t>
         </is>
       </c>
       <c r="E90" s="3" t="n">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="F90" s="3" t="inlineStr">
         <is>
@@ -4695,17 +4667,17 @@
       </c>
       <c r="H90" s="3" t="inlineStr">
         <is>
-          <t>98 x R$ 8909,00</t>
+          <t>64 x R$ 2966,00</t>
         </is>
       </c>
       <c r="I90" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J90" s="3" t="inlineStr">
         <is>
-          <t>Junção</t>
+          <t>VP06</t>
         </is>
       </c>
     </row>
@@ -4722,16 +4694,16 @@
       </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
-          <t>20300,00</t>
+          <t>261200,00</t>
         </is>
       </c>
       <c r="D91" s="3" t="inlineStr">
         <is>
-          <t>10515,00</t>
+          <t>98960,00</t>
         </is>
       </c>
       <c r="E91" s="3" t="n">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="F91" s="3" t="inlineStr">
         <is>
@@ -4740,17 +4712,17 @@
       </c>
       <c r="G91" s="3" t="inlineStr">
         <is>
-          <t>Disponível</t>
+          <t>Indisponível</t>
         </is>
       </c>
       <c r="H91" s="3" t="inlineStr">
         <is>
-          <t>92 x R$ 155,30</t>
+          <t>34 x R$ 9100,00</t>
         </is>
       </c>
       <c r="I91" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J91" s="3" t="inlineStr"/>
@@ -4768,20 +4740,20 @@
       </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
-          <t>27800,00</t>
+          <t>331000,00</t>
         </is>
       </c>
       <c r="D92" s="3" t="inlineStr">
         <is>
-          <t>14390,00</t>
+          <t>164450,00</t>
         </is>
       </c>
       <c r="E92" s="3" t="n">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F92" s="3" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G92" s="3" t="inlineStr">
@@ -4791,15 +4763,19 @@
       </c>
       <c r="H92" s="3" t="inlineStr">
         <is>
-          <t>75 x R$ 261,50</t>
+          <t>82 x R$ 3628,00</t>
         </is>
       </c>
       <c r="I92" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
-        </is>
-      </c>
-      <c r="J92" s="3" t="inlineStr"/>
+          <t>09/05/2025</t>
+        </is>
+      </c>
+      <c r="J92" s="3" t="inlineStr">
+        <is>
+          <t>VP13</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
@@ -4814,20 +4790,20 @@
       </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>28700,00</t>
+          <t>372590,00</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
         <is>
-          <t>17935,00</t>
+          <t>181329,50</t>
         </is>
       </c>
       <c r="E93" s="3" t="n">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="F93" s="3" t="inlineStr">
         <is>
-          <t>Itaú</t>
+          <t>Porto Seguro</t>
         </is>
       </c>
       <c r="G93" s="3" t="inlineStr">
@@ -4837,12 +4813,12 @@
       </c>
       <c r="H93" s="3" t="inlineStr">
         <is>
-          <t>71 x R$ 226,74</t>
+          <t>109 x R$ 3723,00</t>
         </is>
       </c>
       <c r="I93" s="3" t="inlineStr">
         <is>
-          <t>13/04/2025</t>
+          <t>09/05/2025</t>
         </is>
       </c>
       <c r="J93" s="3" t="inlineStr"/>

</xml_diff>